<commit_message>
reset module is writing to RSTCAUSE SFR, reset cause is readable
</commit_message>
<xml_diff>
--- a/docs/sfr_spec.xlsx
+++ b/docs/sfr_spec.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t xml:space="preserve">RSTCON</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t xml:space="preserve">Setting this bit generates a software reset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RSTCAUSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cause of reset. 0: POR reset. 1: External reset. 2: Software reset (SWRST bit was set). 3: Stack overflow/underflow reset. 4: Illegal operand reset.</t>
   </si>
   <si>
     <t xml:space="preserve">TMRCON</t>
@@ -64,6 +70,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -85,9 +92,10 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,6 +108,18 @@
         <bgColor rgb="FF003300"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3465A4"/>
+        <bgColor rgb="FF3366FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF069A2E"/>
+        <bgColor rgb="FF339966"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border diagonalUp="false" diagonalDown="false">
@@ -197,9 +217,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -208,7 +230,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -232,12 +254,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -256,8 +282,68 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Accent 1" xfId="20"/>
+    <cellStyle name="Accent 1 1" xfId="20"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF069A2E"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF3465A4"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -266,13 +352,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C3:J21"/>
+  <dimension ref="C3:J26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="1" t="n">
@@ -334,18 +420,17 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="1" t="n">
-        <f aca="false">C3+1</f>
         <v>1</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="3" t="n">
@@ -374,33 +459,35 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="3"/>
-      <c r="G10" s="8" t="s">
+      <c r="C10" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" customFormat="false" ht="47.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C11" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-    </row>
-    <row r="11" customFormat="false" ht="47.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="1" t="n">
-        <f aca="false">C8+1</f>
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -436,32 +523,31 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="1" t="n">
-        <f aca="false">C13+1</f>
         <v>3</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -501,41 +587,109 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="1" t="n">
+        <f aca="false">C18+1</f>
+        <v>4</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J24" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C26" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="13">
     <mergeCell ref="D3:J3"/>
     <mergeCell ref="D8:J8"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="C10:J10"/>
+    <mergeCell ref="C11:J11"/>
     <mergeCell ref="D13:J13"/>
     <mergeCell ref="C15:J15"/>
     <mergeCell ref="C16:J16"/>
     <mergeCell ref="D18:J18"/>
     <mergeCell ref="C20:J20"/>
     <mergeCell ref="C21:J21"/>
+    <mergeCell ref="D23:J23"/>
+    <mergeCell ref="C25:J25"/>
+    <mergeCell ref="C26:J26"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
timer module working. sfr calculator spreadsheet added.
</commit_message>
<xml_diff>
--- a/docs/sfr_spec.xlsx
+++ b/docs/sfr_spec.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t xml:space="preserve">RSTCON</t>
   </si>
@@ -40,6 +40,12 @@
     <t xml:space="preserve">TMRCON</t>
   </si>
   <si>
+    <t xml:space="preserve">TMRON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMRMODE</t>
+  </si>
+  <si>
     <t xml:space="preserve">PRESCALE</t>
   </si>
   <si>
@@ -53,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">TMROUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH</t>
   </si>
   <si>
     <t xml:space="preserve">Output of the timer’s internal counter</t>
@@ -221,7 +230,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -264,6 +273,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -354,8 +371,8 @@
   </sheetPr>
   <dimension ref="C3:J26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -523,35 +540,37 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
+      <c r="D15" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C16" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="1" t="n">
         <v>3</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -587,28 +606,28 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
+      <c r="C20" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C21" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
+      <c r="C21" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C23" s="1" t="n">
@@ -616,7 +635,7 @@
         <v>4</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
@@ -652,44 +671,44 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C26" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
+      <c r="C25" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C26" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="11">
     <mergeCell ref="D3:J3"/>
     <mergeCell ref="D8:J8"/>
     <mergeCell ref="C10:J10"/>
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="D13:J13"/>
-    <mergeCell ref="C15:J15"/>
-    <mergeCell ref="C16:J16"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="G16:J16"/>
     <mergeCell ref="D18:J18"/>
     <mergeCell ref="C20:J20"/>
     <mergeCell ref="C21:J21"/>
     <mergeCell ref="D23:J23"/>
-    <mergeCell ref="C25:J25"/>
-    <mergeCell ref="C26:J26"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
uart tx works in sim
</commit_message>
<xml_diff>
--- a/docs/sfr_spec.xlsx
+++ b/docs/sfr_spec.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t xml:space="preserve">RSTCON</t>
   </si>
@@ -65,6 +65,45 @@
   </si>
   <si>
     <t xml:space="preserve">Output of the timer’s internal counter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xxx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TXCON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAUD_HILO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">START</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enables the timer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 for 9600, 1 for 115200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set to 1 to begin transmitting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TXREG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data to transmit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TXSTAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUSY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 when transmitter is busy</t>
   </si>
 </sst>
 </file>
@@ -369,13 +408,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C3:J26"/>
+  <dimension ref="C3:J56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D55" activeCellId="0" sqref="D55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="1" t="n">
@@ -696,8 +735,412 @@
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
     </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="1" t="n">
+        <f aca="false">C23+1</f>
+        <v>5</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J29" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="1" t="n">
+        <f aca="false">C28+1</f>
+        <v>6</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C34" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G34" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J34" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="1" t="n">
+        <f aca="false">C33+1</f>
+        <v>7</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G39" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J39" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C40" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C43" s="1" t="n">
+        <f aca="false">C38+1</f>
+        <v>8</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C44" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J44" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C45" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J45" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C46" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J46" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C48" s="1" t="n">
+        <f aca="false">C43+1</f>
+        <v>9</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C49" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E49" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F49" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G49" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H49" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J49" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C50" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C51" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C53" s="1" t="n">
+        <f aca="false">C48+1</f>
+        <v>10</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="8"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C54" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G54" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I54" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J54" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="19">
     <mergeCell ref="D3:J3"/>
     <mergeCell ref="D8:J8"/>
     <mergeCell ref="C10:J10"/>
@@ -709,6 +1152,14 @@
     <mergeCell ref="C20:J20"/>
     <mergeCell ref="C21:J21"/>
     <mergeCell ref="D23:J23"/>
+    <mergeCell ref="D28:J28"/>
+    <mergeCell ref="D33:J33"/>
+    <mergeCell ref="D38:J38"/>
+    <mergeCell ref="D43:J43"/>
+    <mergeCell ref="D48:J48"/>
+    <mergeCell ref="C50:J50"/>
+    <mergeCell ref="C51:J51"/>
+    <mergeCell ref="D53:J53"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
uart rx working in sim, with features (loopback, rx_avail bit cleared on reading)
</commit_message>
<xml_diff>
--- a/docs/sfr_spec.xlsx
+++ b/docs/sfr_spec.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t xml:space="preserve">RSTCON</t>
   </si>
@@ -61,21 +61,33 @@
     <t xml:space="preserve">TMROUT</t>
   </si>
   <si>
+    <t xml:space="preserve">Output of the timer’s internal counter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TMRSTAT</t>
+  </si>
+  <si>
     <t xml:space="preserve">MATCH</t>
   </si>
   <si>
-    <t xml:space="preserve">Output of the timer’s internal counter</t>
+    <t xml:space="preserve">1 when timer counter equals match value</t>
   </si>
   <si>
     <t xml:space="preserve">xxx</t>
   </si>
   <si>
-    <t xml:space="preserve">TXCON</t>
+    <t xml:space="preserve">blah blah blah blah blah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UARTCON</t>
   </si>
   <si>
     <t xml:space="preserve">EN</t>
   </si>
   <si>
+    <t xml:space="preserve">LOOPBACK</t>
+  </si>
+  <si>
     <t xml:space="preserve">BAUD_HILO</t>
   </si>
   <si>
@@ -91,19 +103,28 @@
     <t xml:space="preserve">Set to 1 to begin transmitting</t>
   </si>
   <si>
+    <t xml:space="preserve">UARTSTAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RXBUSY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TXBUSY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 when transmitter is busy</t>
+  </si>
+  <si>
     <t xml:space="preserve">TXREG</t>
   </si>
   <si>
     <t xml:space="preserve">Data to transmit</t>
   </si>
   <si>
-    <t xml:space="preserve">TXSTAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BUSY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 when transmitter is busy</t>
+    <t xml:space="preserve">RXREG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data received</t>
   </si>
 </sst>
 </file>
@@ -408,10 +429,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C3:J56"/>
+  <dimension ref="C3:J71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D55" activeCellId="0" sqref="D55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H86" activeCellId="0" sqref="H86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -719,13 +740,11 @@
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
-      <c r="J25" s="13" t="s">
+      <c r="J25" s="13"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C26" s="14" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="14" t="s">
-        <v>14</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
@@ -741,7 +760,7 @@
         <v>5</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
@@ -785,20 +804,20 @@
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
       <c r="J30" s="13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="14" t="s">
-        <v>14</v>
-      </c>
+      <c r="C31" s="14"/>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
       <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
+      <c r="J31" s="14" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="1" t="n">
@@ -806,7 +825,7 @@
         <v>6</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
@@ -852,12 +871,12 @@
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
       <c r="J35" s="13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
@@ -873,7 +892,7 @@
         <v>7</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
@@ -919,12 +938,12 @@
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
       <c r="J40" s="13" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
@@ -939,15 +958,15 @@
         <f aca="false">C38+1</f>
         <v>8</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
+      <c r="D43" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="3" t="n">
@@ -976,51 +995,41 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="13" t="s">
-        <v>17</v>
-      </c>
+      <c r="C45" s="13"/>
       <c r="D45" s="13"/>
       <c r="E45" s="13"/>
       <c r="F45" s="13"/>
       <c r="G45" s="13"/>
       <c r="H45" s="13"/>
-      <c r="I45" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="J45" s="13" t="s">
-        <v>19</v>
-      </c>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
     </row>
     <row r="46" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
       <c r="F46" s="14"/>
       <c r="G46" s="14"/>
       <c r="H46" s="14"/>
-      <c r="I46" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J46" s="14" t="s">
-        <v>22</v>
-      </c>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="1" t="n">
         <f aca="false">C43+1</f>
         <v>9</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
+      <c r="D48" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="3" t="n">
@@ -1049,22 +1058,18 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="13" t="s">
-        <v>23</v>
-      </c>
+      <c r="C50" s="13"/>
       <c r="D50" s="13"/>
       <c r="E50" s="13"/>
       <c r="F50" s="13"/>
       <c r="G50" s="13"/>
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
-      <c r="J50" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="J50" s="13"/>
+    </row>
+    <row r="51" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="14" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
@@ -1076,18 +1081,18 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="1" t="n">
-        <f aca="false">C48+1</f>
-        <v>10</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E53" s="8"/>
-      <c r="F53" s="8"/>
-      <c r="G53" s="8"/>
-      <c r="H53" s="8"/>
-      <c r="I53" s="8"/>
-      <c r="J53" s="8"/>
+        <f aca="false">C38+1</f>
+        <v>8</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="3" t="n">
@@ -1116,31 +1121,240 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C55" s="13"/>
+      <c r="C55" s="13" t="s">
+        <v>20</v>
+      </c>
       <c r="D55" s="13"/>
       <c r="E55" s="13"/>
       <c r="F55" s="13"/>
       <c r="G55" s="13"/>
-      <c r="H55" s="13"/>
-      <c r="I55" s="13"/>
+      <c r="H55" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I55" s="13" t="s">
+        <v>22</v>
+      </c>
       <c r="J55" s="13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="14"/>
+      <c r="C56" s="14" t="s">
+        <v>24</v>
+      </c>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
       <c r="F56" s="14"/>
       <c r="G56" s="14"/>
       <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
+      <c r="I56" s="14" t="s">
+        <v>25</v>
+      </c>
       <c r="J56" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C58" s="1" t="n">
+        <f aca="false">C53+1</f>
+        <v>9</v>
+      </c>
+      <c r="D58" s="8" t="s">
         <v>27</v>
       </c>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C59" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F59" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G59" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H59" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J59" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="J60" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="14"/>
+      <c r="J61" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C63" s="1" t="n">
+        <f aca="false">C58+1</f>
+        <v>10</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C64" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F64" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G64" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H64" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I64" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J64" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C65" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C66" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
+      <c r="J66" s="14"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C68" s="1" t="n">
+        <f aca="false">C63+1</f>
+        <v>11</v>
+      </c>
+      <c r="D68" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
+      <c r="J68" s="8"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C69" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F69" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G69" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H69" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="I69" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J69" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="13"/>
+      <c r="J70" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="24">
     <mergeCell ref="D3:J3"/>
     <mergeCell ref="D8:J8"/>
     <mergeCell ref="C10:J10"/>
@@ -1152,14 +1366,19 @@
     <mergeCell ref="C20:J20"/>
     <mergeCell ref="C21:J21"/>
     <mergeCell ref="D23:J23"/>
+    <mergeCell ref="C25:J25"/>
+    <mergeCell ref="C26:J26"/>
     <mergeCell ref="D28:J28"/>
     <mergeCell ref="D33:J33"/>
     <mergeCell ref="D38:J38"/>
     <mergeCell ref="D43:J43"/>
     <mergeCell ref="D48:J48"/>
-    <mergeCell ref="C50:J50"/>
-    <mergeCell ref="C51:J51"/>
     <mergeCell ref="D53:J53"/>
+    <mergeCell ref="D58:J58"/>
+    <mergeCell ref="D63:J63"/>
+    <mergeCell ref="C65:J65"/>
+    <mergeCell ref="C66:J66"/>
+    <mergeCell ref="D68:J68"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>